<commit_message>
Update PowerPoint Group IDs.
</commit_message>
<xml_diff>
--- a/PowerPoint/PowerPoint on the web Ribbon IDs.xlsx
+++ b/PowerPoint/PowerPoint on the web Ribbon IDs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garycha.REDMOND\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garycha.REDMOND\Downloads\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4065F696-CA42-4EC5-A9F9-43083F156073}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DA99A6-F87B-43F7-BC6E-68745610FAE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="27977" windowHeight="18274" xr2:uid="{B2780061-72EF-4F7B-A02F-E2956A27150E}"/>
+    <workbookView xWindow="61425" yWindow="19155" windowWidth="11910" windowHeight="3300" xr2:uid="{B2780061-72EF-4F7B-A02F-E2956A27150E}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="254">
   <si>
     <t>EffectOptionsMenu</t>
   </si>
@@ -596,9 +596,6 @@
     <t>GroupTransitionEffectOptionsOnline</t>
   </si>
   <si>
-    <t>GroupTransitionAllSlidesOnline</t>
-  </si>
-  <si>
     <t>GroupAnimations</t>
   </si>
   <si>
@@ -729,9 +726,6 @@
   </si>
   <si>
     <t>GroupInsertText</t>
-  </si>
-  <si>
-    <t>GroupOfficeExtension</t>
   </si>
   <si>
     <t>GroupSlides2</t>
@@ -873,8 +867,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{087CA890-B44F-4758-9FF5-BFB6BDFF4635}" name="Table214" displayName="Table214" ref="A1:B53" totalsRowShown="0">
-  <autoFilter ref="A1:B53" xr:uid="{8BCC57C3-9FD3-4C59-86B5-B4910DB6E1B6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{087CA890-B44F-4758-9FF5-BFB6BDFF4635}" name="Table214" displayName="Table214" ref="A1:B51" totalsRowShown="0">
+  <autoFilter ref="A1:B51" xr:uid="{8BCC57C3-9FD3-4C59-86B5-B4910DB6E1B6}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B51">
+    <sortCondition ref="B1:B51"/>
+  </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{BC1E194D-05A9-481A-9038-4A887ED7F39B}" name="PowerPoint on the Web GoupID"/>
     <tableColumn id="2" xr3:uid="{69BFACFF-6820-4CAC-9BA7-E8B28D15B46C}" name="Ribbon Tab ID"/>
@@ -884,8 +881,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{ECB74D88-61DB-4B2B-806F-3679FB9ECD87}" name="Table115" displayName="Table115" ref="A1:B57" totalsRowShown="0">
-  <autoFilter ref="A1:B57" xr:uid="{04878540-34C7-4048-BFE3-2C42DA047434}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{ECB74D88-61DB-4B2B-806F-3679FB9ECD87}" name="Table115" displayName="Table115" ref="A1:B54" totalsRowShown="0">
+  <autoFilter ref="A1:B54" xr:uid="{04878540-34C7-4048-BFE3-2C42DA047434}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B54">
+    <sortCondition ref="B1:B54"/>
+  </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1B4FB867-866F-49B5-BDBE-0281BFEB4D86}" name="PowerPoint on the Web GoupID"/>
     <tableColumn id="2" xr3:uid="{620B0D22-3B69-4707-9515-AADD83DF2406}" name="Ribbon Tab ID"/>
@@ -1221,7 +1221,7 @@
   <dimension ref="A1:B172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1233,10 +1233,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
@@ -1489,7 +1489,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B33" t="s">
         <v>20</v>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B34" t="s">
         <v>20</v>
@@ -1593,7 +1593,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B46" t="s">
         <v>49</v>
@@ -1601,7 +1601,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B47" t="s">
         <v>49</v>
@@ -1609,7 +1609,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B48" t="s">
         <v>49</v>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B49" t="s">
         <v>49</v>
@@ -1625,7 +1625,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B50" t="s">
         <v>49</v>
@@ -1633,7 +1633,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B51" t="s">
         <v>49</v>
@@ -1753,7 +1753,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B66" t="s">
         <v>49</v>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B68" t="s">
         <v>49</v>
@@ -1833,7 +1833,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B76" t="s">
         <v>49</v>
@@ -1857,7 +1857,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B79" t="s">
         <v>49</v>
@@ -2353,7 +2353,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A141" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B141" t="s">
         <v>132</v>
@@ -2361,7 +2361,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A142" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B142" t="s">
         <v>132</v>
@@ -2385,7 +2385,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A145" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B145" t="s">
         <v>132</v>
@@ -2457,7 +2457,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A154" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B154" t="s">
         <v>148</v>
@@ -2617,10 +2617,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CC975D7-E569-4A80-93F7-512D5D356E85}">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2632,186 +2632,186 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B1" t="s">
         <v>237</v>
-      </c>
-      <c r="B1" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>189</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>176</v>
+        <v>220</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>177</v>
+        <v>221</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="B18" t="s">
-        <v>148</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="B19" t="s">
-        <v>148</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="B20" t="s">
-        <v>148</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="B21" t="s">
-        <v>148</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="B22" t="s">
-        <v>188</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="B23" t="s">
-        <v>188</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.4">
@@ -2819,7 +2819,7 @@
         <v>190</v>
       </c>
       <c r="B24" t="s">
-        <v>188</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.4">
@@ -2864,194 +2864,178 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B30" t="s">
-        <v>109</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B31" t="s">
-        <v>151</v>
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B32" t="s">
-        <v>151</v>
+        <v>200</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B33" t="s">
-        <v>151</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="B34" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="B35" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="B36" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="B37" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
+        <v>207</v>
+      </c>
+      <c r="B38" t="s">
         <v>205</v>
-      </c>
-      <c r="B38" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B42" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B43" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B44" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="B45" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>214</v>
+        <v>185</v>
       </c>
       <c r="B46" t="s">
-        <v>206</v>
+        <v>148</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
       <c r="B47" t="s">
-        <v>216</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>217</v>
+        <v>184</v>
       </c>
       <c r="B48" t="s">
-        <v>216</v>
+        <v>148</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
       <c r="B49" t="s">
-        <v>216</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>219</v>
+        <v>197</v>
       </c>
       <c r="B50" t="s">
-        <v>216</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B51" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A52" t="s">
-        <v>221</v>
-      </c>
-      <c r="B52" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A53" t="s">
-        <v>222</v>
-      </c>
-      <c r="B53" t="s">
-        <v>220</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -3064,10 +3048,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D6CCE0-1E97-4D8F-8F6B-03C1E93F1C98}">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3079,63 +3063,63 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B1" t="s">
         <v>237</v>
-      </c>
-      <c r="B1" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>221</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B8" t="s">
         <v>49</v>
@@ -3143,7 +3127,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B9" t="s">
         <v>49</v>
@@ -3151,7 +3135,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B10" t="s">
         <v>49</v>
@@ -3159,7 +3143,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B11" t="s">
         <v>49</v>
@@ -3167,55 +3151,55 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>223</v>
+        <v>171</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>224</v>
+        <v>172</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>225</v>
+        <v>173</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>226</v>
+        <v>174</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>227</v>
+        <v>175</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>228</v>
+        <v>176</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B18" t="s">
         <v>94</v>
@@ -3223,7 +3207,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B19" t="s">
         <v>94</v>
@@ -3231,7 +3215,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B20" t="s">
         <v>94</v>
@@ -3239,7 +3223,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="B21" t="s">
         <v>94</v>
@@ -3247,7 +3231,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B22" t="s">
         <v>94</v>
@@ -3255,7 +3239,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B23" t="s">
         <v>94</v>
@@ -3263,71 +3247,71 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>178</v>
+        <v>228</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>179</v>
+        <v>229</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>180</v>
+        <v>230</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>181</v>
+        <v>231</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>183</v>
+        <v>232</v>
       </c>
       <c r="B28" t="s">
-        <v>148</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B29" t="s">
-        <v>148</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B30" t="s">
-        <v>188</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B31" t="s">
-        <v>188</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B32" t="s">
         <v>109</v>
@@ -3335,7 +3319,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B33" t="s">
         <v>109</v>
@@ -3343,194 +3327,170 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="B34" t="s">
-        <v>109</v>
+        <v>200</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="B35" t="s">
-        <v>109</v>
+        <v>200</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>195</v>
+        <v>214</v>
       </c>
       <c r="B36" t="s">
-        <v>109</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="B37" t="s">
-        <v>109</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>198</v>
+        <v>217</v>
       </c>
       <c r="B38" t="s">
-        <v>151</v>
+        <v>215</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>199</v>
+        <v>218</v>
       </c>
       <c r="B39" t="s">
-        <v>151</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
       <c r="B40" t="s">
-        <v>151</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B41" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B42" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
+        <v>208</v>
+      </c>
+      <c r="B43" t="s">
         <v>205</v>
-      </c>
-      <c r="B43" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B44" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B45" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B46" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="B47" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B48" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B49" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>236</v>
+        <v>183</v>
       </c>
       <c r="B50" t="s">
-        <v>206</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>213</v>
+        <v>184</v>
       </c>
       <c r="B51" t="s">
-        <v>206</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="B52" t="s">
-        <v>206</v>
+        <v>151</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="B53" t="s">
-        <v>216</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="B54" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A55" t="s">
-        <v>218</v>
-      </c>
-      <c r="B55" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A56" t="s">
-        <v>219</v>
-      </c>
-      <c r="B56" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A57" t="s">
-        <v>222</v>
-      </c>
-      <c r="B57" t="s">
-        <v>220</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -3542,46 +3502,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Recording xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Recording>
-    <OXOCommonsPost xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </OXOCommonsPost>
-    <Last_x0020_Modified_x0020_by xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Last_x0020_Modified_x0020_by>
-    <Status xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">One Pager</Status>
-    <Document_x0020_Purpose xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">Informational</Document_x0020_Purpose>
-    <MediaServiceKeyPoints xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Initiatives xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4"/>
-    <OneNoteFluid_Labels xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4" xsi:nil="true"/>
-    <SpecialTopics xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4" xsi:nil="true"/>
-    <OneNoteFluid_FileOrder xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">=</OneNoteFluid_FileOrder>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CD401524DC532D42A0E0ED886331A72B" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d2008d1df3c02478111991a3195c98a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f577acbf-5b0b-4b4f-9948-268e97f8d3a4" xmlns:ns3="b1e4d6ee-9f6f-43f8-a618-24f3d84da28f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="999d8bb98d9b3ee138da5d49232ece6d" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3940,10 +3860,62 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Recording xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Recording>
+    <OXOCommonsPost xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </OXOCommonsPost>
+    <Last_x0020_Modified_x0020_by xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Last_x0020_Modified_x0020_by>
+    <Status xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">One Pager</Status>
+    <Document_x0020_Purpose xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">Informational</Document_x0020_Purpose>
+    <MediaServiceKeyPoints xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Initiatives xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4"/>
+    <OneNoteFluid_Labels xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4" xsi:nil="true"/>
+    <SpecialTopics xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4" xsi:nil="true"/>
+    <OneNoteFluid_FileOrder xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">=</OneNoteFluid_FileOrder>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47CABA21-83B6-4095-9E22-101E08B44D5A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7B4FB74-6111-4727-8258-27F1844C7822}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="f577acbf-5b0b-4b4f-9948-268e97f8d3a4"/>
+    <ds:schemaRef ds:uri="b1e4d6ee-9f6f-43f8-a618-24f3d84da28f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3967,21 +3939,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7B4FB74-6111-4727-8258-27F1844C7822}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47CABA21-83B6-4095-9E22-101E08B44D5A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="f577acbf-5b0b-4b4f-9948-268e97f8d3a4"/>
-    <ds:schemaRef ds:uri="b1e4d6ee-9f6f-43f8-a618-24f3d84da28f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Remove unsupported control ID.
</commit_message>
<xml_diff>
--- a/PowerPoint/PowerPoint on the web Ribbon IDs.xlsx
+++ b/PowerPoint/PowerPoint on the web Ribbon IDs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23704"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garycha.REDMOND\Downloads\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garycha.REDMOND\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DA99A6-F87B-43F7-BC6E-68745610FAE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374948B0-B694-4ABE-833E-F54F0305B314}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61425" yWindow="19155" windowWidth="11910" windowHeight="3300" xr2:uid="{B2780061-72EF-4F7B-A02F-E2956A27150E}"/>
+    <workbookView xWindow="48480" yWindow="10860" windowWidth="38640" windowHeight="21390" activeTab="2" xr2:uid="{B2780061-72EF-4F7B-A02F-E2956A27150E}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="252">
   <si>
     <t>EffectOptionsMenu</t>
   </si>
@@ -558,12 +558,6 @@
   </si>
   <si>
     <t>GroupVoiceTools</t>
-  </si>
-  <si>
-    <t>GroupUndoOnline</t>
-  </si>
-  <si>
-    <t>GroupDeleteOnline</t>
   </si>
   <si>
     <t>GroupDesignerHome</t>
@@ -867,10 +861,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{087CA890-B44F-4758-9FF5-BFB6BDFF4635}" name="Table214" displayName="Table214" ref="A1:B51" totalsRowShown="0">
-  <autoFilter ref="A1:B51" xr:uid="{8BCC57C3-9FD3-4C59-86B5-B4910DB6E1B6}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B51">
-    <sortCondition ref="B1:B51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{087CA890-B44F-4758-9FF5-BFB6BDFF4635}" name="Table214" displayName="Table214" ref="A1:B49" totalsRowShown="0">
+  <autoFilter ref="A1:B49" xr:uid="{8BCC57C3-9FD3-4C59-86B5-B4910DB6E1B6}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B49">
+    <sortCondition ref="B1:B49"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{BC1E194D-05A9-481A-9038-4A887ED7F39B}" name="PowerPoint on the Web GoupID"/>
@@ -881,10 +875,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{ECB74D88-61DB-4B2B-806F-3679FB9ECD87}" name="Table115" displayName="Table115" ref="A1:B54" totalsRowShown="0">
-  <autoFilter ref="A1:B54" xr:uid="{04878540-34C7-4048-BFE3-2C42DA047434}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B54">
-    <sortCondition ref="B1:B54"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{ECB74D88-61DB-4B2B-806F-3679FB9ECD87}" name="Table115" displayName="Table115" ref="A1:B52" totalsRowShown="0">
+  <autoFilter ref="A1:B52" xr:uid="{04878540-34C7-4048-BFE3-2C42DA047434}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B52">
+    <sortCondition ref="B1:B52"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1B4FB867-866F-49B5-BDBE-0281BFEB4D86}" name="PowerPoint on the Web GoupID"/>
@@ -1220,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79AED04-8231-4CCF-B0CD-97145ACF0837}">
   <dimension ref="A1:B172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1233,10 +1227,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
@@ -1489,7 +1483,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B33" t="s">
         <v>20</v>
@@ -1497,7 +1491,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B34" t="s">
         <v>20</v>
@@ -1593,7 +1587,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B46" t="s">
         <v>49</v>
@@ -1601,7 +1595,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B47" t="s">
         <v>49</v>
@@ -1609,7 +1603,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B48" t="s">
         <v>49</v>
@@ -1617,7 +1611,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B49" t="s">
         <v>49</v>
@@ -1625,7 +1619,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B50" t="s">
         <v>49</v>
@@ -1633,7 +1627,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B51" t="s">
         <v>49</v>
@@ -1753,7 +1747,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B66" t="s">
         <v>49</v>
@@ -1769,7 +1763,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B68" t="s">
         <v>49</v>
@@ -1833,7 +1827,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B76" t="s">
         <v>49</v>
@@ -1857,7 +1851,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B79" t="s">
         <v>49</v>
@@ -2353,7 +2347,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A141" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B141" t="s">
         <v>132</v>
@@ -2361,7 +2355,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A142" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B142" t="s">
         <v>132</v>
@@ -2385,7 +2379,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A145" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B145" t="s">
         <v>132</v>
@@ -2457,7 +2451,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A154" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B154" t="s">
         <v>148</v>
@@ -2617,10 +2611,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CC975D7-E569-4A80-93F7-512D5D356E85}">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2632,39 +2626,39 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" t="s">
         <v>235</v>
-      </c>
-      <c r="B1" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -2672,7 +2666,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -2680,7 +2674,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -2688,7 +2682,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -2696,7 +2690,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -2704,26 +2698,26 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
@@ -2736,7 +2730,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B14" t="s">
         <v>49</v>
@@ -2744,7 +2738,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B15" t="s">
         <v>49</v>
@@ -2752,7 +2746,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B16" t="s">
         <v>49</v>
@@ -2760,7 +2754,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B17" t="s">
         <v>49</v>
@@ -2768,7 +2762,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B18" t="s">
         <v>49</v>
@@ -2776,7 +2770,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B19" t="s">
         <v>49</v>
@@ -2784,7 +2778,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B20" t="s">
         <v>49</v>
@@ -2792,26 +2786,26 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.4">
@@ -2848,26 +2842,26 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B28" t="s">
-        <v>109</v>
+        <v>198</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B29" t="s">
-        <v>109</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B30" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.4">
@@ -2875,31 +2869,31 @@
         <v>201</v>
       </c>
       <c r="B31" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="B32" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="B33" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B34" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.4">
@@ -2907,23 +2901,23 @@
         <v>216</v>
       </c>
       <c r="B35" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="B36" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="B37" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.4">
@@ -2931,7 +2925,7 @@
         <v>207</v>
       </c>
       <c r="B38" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.4">
@@ -2939,7 +2933,7 @@
         <v>208</v>
       </c>
       <c r="B39" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.4">
@@ -2947,7 +2941,7 @@
         <v>209</v>
       </c>
       <c r="B40" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.4">
@@ -2955,44 +2949,44 @@
         <v>210</v>
       </c>
       <c r="B41" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B42" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B43" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="B44" t="s">
-        <v>205</v>
+        <v>148</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="B45" t="s">
-        <v>205</v>
+        <v>148</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B46" t="s">
         <v>148</v>
@@ -3000,18 +2994,18 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="B47" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="B48" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.4">
@@ -3019,22 +3013,6 @@
         <v>196</v>
       </c>
       <c r="B49" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A50" t="s">
-        <v>197</v>
-      </c>
-      <c r="B50" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A51" t="s">
-        <v>198</v>
-      </c>
-      <c r="B51" t="s">
         <v>151</v>
       </c>
     </row>
@@ -3048,10 +3026,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D6CCE0-1E97-4D8F-8F6B-03C1E93F1C98}">
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3063,31 +3041,31 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" t="s">
         <v>235</v>
-      </c>
-      <c r="B1" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -3095,7 +3073,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -3103,7 +3081,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -3111,10 +3089,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
@@ -3183,18 +3161,18 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>175</v>
+        <v>220</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>176</v>
+        <v>221</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.4">
@@ -3271,18 +3249,18 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>232</v>
+        <v>189</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.4">
@@ -3295,7 +3273,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B30" t="s">
         <v>109</v>
@@ -3303,7 +3281,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B31" t="s">
         <v>109</v>
@@ -3311,42 +3289,42 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B32" t="s">
-        <v>109</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="B33" t="s">
-        <v>109</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="B34" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="B35" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B36" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.4">
@@ -3354,31 +3332,31 @@
         <v>216</v>
       </c>
       <c r="B37" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="B38" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="B39" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B40" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.4">
@@ -3386,7 +3364,7 @@
         <v>206</v>
       </c>
       <c r="B41" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.4">
@@ -3394,7 +3372,7 @@
         <v>207</v>
       </c>
       <c r="B42" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.4">
@@ -3402,7 +3380,7 @@
         <v>208</v>
       </c>
       <c r="B43" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.4">
@@ -3410,86 +3388,70 @@
         <v>209</v>
       </c>
       <c r="B44" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>210</v>
+        <v>232</v>
       </c>
       <c r="B45" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B46" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>234</v>
+        <v>211</v>
       </c>
       <c r="B47" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>212</v>
+        <v>181</v>
       </c>
       <c r="B48" t="s">
-        <v>205</v>
+        <v>148</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>213</v>
+        <v>182</v>
       </c>
       <c r="B49" t="s">
-        <v>205</v>
+        <v>148</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="B50" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="B51" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="B52" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A53" t="s">
-        <v>198</v>
-      </c>
-      <c r="B53" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A54" t="s">
-        <v>233</v>
-      </c>
-      <c r="B54" t="s">
         <v>151</v>
       </c>
     </row>
@@ -3502,6 +3464,46 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Recording xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Recording>
+    <OXOCommonsPost xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </OXOCommonsPost>
+    <Last_x0020_Modified_x0020_by xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Last_x0020_Modified_x0020_by>
+    <Status xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">One Pager</Status>
+    <Document_x0020_Purpose xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">Informational</Document_x0020_Purpose>
+    <MediaServiceKeyPoints xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Initiatives xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4"/>
+    <OneNoteFluid_Labels xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4" xsi:nil="true"/>
+    <SpecialTopics xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4" xsi:nil="true"/>
+    <OneNoteFluid_FileOrder xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">=</OneNoteFluid_FileOrder>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CD401524DC532D42A0E0ED886331A72B" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d2008d1df3c02478111991a3195c98a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f577acbf-5b0b-4b4f-9948-268e97f8d3a4" xmlns:ns3="b1e4d6ee-9f6f-43f8-a618-24f3d84da28f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="999d8bb98d9b3ee138da5d49232ece6d" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3860,62 +3862,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Recording xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Recording>
-    <OXOCommonsPost xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </OXOCommonsPost>
-    <Last_x0020_Modified_x0020_by xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Last_x0020_Modified_x0020_by>
-    <Status xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">One Pager</Status>
-    <Document_x0020_Purpose xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">Informational</Document_x0020_Purpose>
-    <MediaServiceKeyPoints xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Initiatives xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4"/>
-    <OneNoteFluid_Labels xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4" xsi:nil="true"/>
-    <SpecialTopics xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4" xsi:nil="true"/>
-    <OneNoteFluid_FileOrder xmlns="f577acbf-5b0b-4b4f-9948-268e97f8d3a4">=</OneNoteFluid_FileOrder>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7B4FB74-6111-4727-8258-27F1844C7822}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47CABA21-83B6-4095-9E22-101E08B44D5A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="f577acbf-5b0b-4b4f-9948-268e97f8d3a4"/>
-    <ds:schemaRef ds:uri="b1e4d6ee-9f6f-43f8-a618-24f3d84da28f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3939,9 +3889,21 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47CABA21-83B6-4095-9E22-101E08B44D5A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7B4FB74-6111-4727-8258-27F1844C7822}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="f577acbf-5b0b-4b4f-9948-268e97f8d3a4"/>
+    <ds:schemaRef ds:uri="b1e4d6ee-9f6f-43f8-a618-24f3d84da28f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>